<commit_message>
Pequeño error encontrado en al escribir los datos en el reporte pequeño, falta hacer que se muestren IP en el IP Report y darle formato.
</commit_message>
<xml_diff>
--- a/results_IP 2.xlsx
+++ b/results_IP 2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dicofra1-my.sharepoint.com/personal/angel_liceaga_dicofra_com_mx/Documents/Documentos/Progra/CSOC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09DA4CD0-79AB-4F8B-A402-444855C35032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{09DA4CD0-79AB-4F8B-A402-444855C35032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECF20DD-2173-4CF1-862C-D9CEB3B26442}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_IP" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="233">
   <si>
     <t>ipAddress</t>
   </si>
@@ -378,12 +378,357 @@
   </si>
   <si>
     <t>tci.ir</t>
+  </si>
+  <si>
+    <t>continentCode</t>
+  </si>
+  <si>
+    <t>continentName</t>
+  </si>
+  <si>
+    <t>countryName</t>
+  </si>
+  <si>
+    <t>isEuMember</t>
+  </si>
+  <si>
+    <t>currencyCode</t>
+  </si>
+  <si>
+    <t>currencyName</t>
+  </si>
+  <si>
+    <t>phonePrefix</t>
+  </si>
+  <si>
+    <t>languages</t>
+  </si>
+  <si>
+    <t>stateProv</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>geonameId</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>gmtOffset</t>
+  </si>
+  <si>
+    <t>timeZone</t>
+  </si>
+  <si>
+    <t>weatherCode</t>
+  </si>
+  <si>
+    <t>asNumber</t>
+  </si>
+  <si>
+    <t>asName</t>
+  </si>
+  <si>
+    <t>organization</t>
+  </si>
+  <si>
+    <t>isCrawler</t>
+  </si>
+  <si>
+    <t>isProxy</t>
+  </si>
+  <si>
+    <t>threatLevel</t>
+  </si>
+  <si>
+    <t>stateProvCode</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>threatDetails</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>TWD</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>886</t>
+  </si>
+  <si>
+    <t>['zh-TW', 'zh', 'nan', 'hak']</t>
+  </si>
+  <si>
+    <t>Taipei City</t>
+  </si>
+  <si>
+    <t>Neihu District</t>
+  </si>
+  <si>
+    <t>Asia/Taipei</t>
+  </si>
+  <si>
+    <t>TWXX5215</t>
+  </si>
+  <si>
+    <t>HINET</t>
+  </si>
+  <si>
+    <t>Chunghwa Telecom Co., Ltd.</t>
+  </si>
+  <si>
+    <t>corporate</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>THB</t>
+  </si>
+  <si>
+    <t>Baht</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>['th', 'en']</t>
+  </si>
+  <si>
+    <t>Bangkok</t>
+  </si>
+  <si>
+    <t>Samphanthawong</t>
+  </si>
+  <si>
+    <t>Samphanthawong (Khwaeng Bang Rak)</t>
+  </si>
+  <si>
+    <t>Asia/Bangkok</t>
+  </si>
+  <si>
+    <t>THXX0581</t>
+  </si>
+  <si>
+    <t>CAT-IDC-4bytenet-AS-AP</t>
+  </si>
+  <si>
+    <t>Cat-Bb</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>10100</t>
+  </si>
+  <si>
+    <t>['attack-source', 'attack-target:web']</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>Yen</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>['ja']</t>
+  </si>
+  <si>
+    <t>Ōsaka</t>
+  </si>
+  <si>
+    <t>Osaka-shi</t>
+  </si>
+  <si>
+    <t>Osaka (Chuo Ward)</t>
+  </si>
+  <si>
+    <t>Asia/Tokyo</t>
+  </si>
+  <si>
+    <t>JAXX0071</t>
+  </si>
+  <si>
+    <t>OPTAGE OPTAGE Inc.</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>540-0002</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>['en-US', 'es-US', 'haw', 'fr']</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Montgomery</t>
+  </si>
+  <si>
+    <t>Moraine</t>
+  </si>
+  <si>
+    <t>America/New_York</t>
+  </si>
+  <si>
+    <t>USOH1188</t>
+  </si>
+  <si>
+    <t>TWC-10796-MIDWEST</t>
+  </si>
+  <si>
+    <t>Spectrum</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>45439</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>['en-GB', 'cy-GB', 'gd']</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Greater London</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Europe/London</t>
+  </si>
+  <si>
+    <t>UKXX0085</t>
+  </si>
+  <si>
+    <t>AS5413</t>
+  </si>
+  <si>
+    <t>Daisy</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>W1B</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>['cmn', 'en-SG', 'ms-SG', 'ta-SG', 'zh-SG']</t>
+  </si>
+  <si>
+    <t>Singapore (Pioneer)</t>
+  </si>
+  <si>
+    <t>Asia/Singapore</t>
+  </si>
+  <si>
+    <t>SNXX0006</t>
+  </si>
+  <si>
+    <t>DIGITALOCEAN-ASN</t>
+  </si>
+  <si>
+    <t>DigitalOcean, LLC</t>
+  </si>
+  <si>
+    <t>hosting</t>
+  </si>
+  <si>
+    <t>627753</t>
+  </si>
+  <si>
+    <t>Taipei</t>
+  </si>
+  <si>
+    <t>TWXX0021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -959,7 +1304,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -988,6 +1333,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1362,11 +1713,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A2:A6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2088,7 +2439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>18</v>
       </c>
@@ -2135,7 +2486,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>19</v>
       </c>
@@ -2180,7 +2531,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>20</v>
       </c>
@@ -2225,18 +2576,1299 @@
         <v>46</v>
       </c>
     </row>
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="O39" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="P39" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q39" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="S39" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="T39" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="U39" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="V39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W39" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="X39" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="Y39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z39" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA39" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB39" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC39" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>146</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>147</v>
+      </c>
+      <c r="G40" t="s">
+        <v>148</v>
+      </c>
+      <c r="H40" t="s">
+        <v>149</v>
+      </c>
+      <c r="I40" t="s">
+        <v>150</v>
+      </c>
+      <c r="J40" t="s">
+        <v>146</v>
+      </c>
+      <c r="K40" t="s">
+        <v>151</v>
+      </c>
+      <c r="L40" t="s">
+        <v>152</v>
+      </c>
+      <c r="M40">
+        <v>1671467</v>
+      </c>
+      <c r="N40">
+        <v>25.068899999999999</v>
+      </c>
+      <c r="O40">
+        <v>121.59099999999999</v>
+      </c>
+      <c r="P40">
+        <v>8</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>153</v>
+      </c>
+      <c r="R40" t="s">
+        <v>154</v>
+      </c>
+      <c r="S40">
+        <v>3462</v>
+      </c>
+      <c r="T40" t="s">
+        <v>155</v>
+      </c>
+      <c r="U40" t="s">
+        <v>156</v>
+      </c>
+      <c r="V40" t="s">
+        <v>157</v>
+      </c>
+      <c r="W40" t="s">
+        <v>41</v>
+      </c>
+      <c r="X40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" t="s">
+        <v>148</v>
+      </c>
+      <c r="H41" t="s">
+        <v>149</v>
+      </c>
+      <c r="I41" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" t="s">
+        <v>146</v>
+      </c>
+      <c r="K41" t="s">
+        <v>151</v>
+      </c>
+      <c r="L41" t="s">
+        <v>152</v>
+      </c>
+      <c r="M41">
+        <v>1671467</v>
+      </c>
+      <c r="N41">
+        <v>25.068899999999999</v>
+      </c>
+      <c r="O41">
+        <v>121.59099999999999</v>
+      </c>
+      <c r="P41">
+        <v>8</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>153</v>
+      </c>
+      <c r="R41" t="s">
+        <v>154</v>
+      </c>
+      <c r="S41">
+        <v>3462</v>
+      </c>
+      <c r="T41" t="s">
+        <v>155</v>
+      </c>
+      <c r="U41" t="s">
+        <v>156</v>
+      </c>
+      <c r="V41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W41" t="s">
+        <v>41</v>
+      </c>
+      <c r="X41" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" t="s">
+        <v>161</v>
+      </c>
+      <c r="H42" t="s">
+        <v>162</v>
+      </c>
+      <c r="I42" t="s">
+        <v>163</v>
+      </c>
+      <c r="J42" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42" t="s">
+        <v>165</v>
+      </c>
+      <c r="L42" t="s">
+        <v>166</v>
+      </c>
+      <c r="M42">
+        <v>1606640</v>
+      </c>
+      <c r="N42">
+        <v>13.726699999999999</v>
+      </c>
+      <c r="O42">
+        <v>100.515</v>
+      </c>
+      <c r="P42">
+        <v>7</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>167</v>
+      </c>
+      <c r="R42" t="s">
+        <v>168</v>
+      </c>
+      <c r="S42">
+        <v>131090</v>
+      </c>
+      <c r="T42" t="s">
+        <v>169</v>
+      </c>
+      <c r="U42" t="s">
+        <v>170</v>
+      </c>
+      <c r="V42" t="s">
+        <v>157</v>
+      </c>
+      <c r="X42" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>144</v>
+      </c>
+      <c r="B43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" t="s">
+        <v>179</v>
+      </c>
+      <c r="J43" t="s">
+        <v>180</v>
+      </c>
+      <c r="K43" t="s">
+        <v>181</v>
+      </c>
+      <c r="L43" t="s">
+        <v>182</v>
+      </c>
+      <c r="M43">
+        <v>1853909</v>
+      </c>
+      <c r="N43">
+        <v>34.692900000000002</v>
+      </c>
+      <c r="O43">
+        <v>135.53</v>
+      </c>
+      <c r="P43">
+        <v>9</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>183</v>
+      </c>
+      <c r="R43" t="s">
+        <v>184</v>
+      </c>
+      <c r="S43">
+        <v>17511</v>
+      </c>
+      <c r="T43" t="s">
+        <v>185</v>
+      </c>
+      <c r="U43" t="s">
+        <v>52</v>
+      </c>
+      <c r="V43" t="s">
+        <v>157</v>
+      </c>
+      <c r="W43" t="s">
+        <v>52</v>
+      </c>
+      <c r="X43" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y43" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>188</v>
+      </c>
+      <c r="B44" t="s">
+        <v>189</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>190</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>191</v>
+      </c>
+      <c r="G44" t="s">
+        <v>148</v>
+      </c>
+      <c r="H44" t="s">
+        <v>192</v>
+      </c>
+      <c r="I44" t="s">
+        <v>193</v>
+      </c>
+      <c r="J44" t="s">
+        <v>194</v>
+      </c>
+      <c r="K44" t="s">
+        <v>195</v>
+      </c>
+      <c r="L44" t="s">
+        <v>196</v>
+      </c>
+      <c r="M44">
+        <v>4518661</v>
+      </c>
+      <c r="N44">
+        <v>39.7211</v>
+      </c>
+      <c r="O44">
+        <v>-84.209599999999995</v>
+      </c>
+      <c r="P44">
+        <v>-4</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>197</v>
+      </c>
+      <c r="R44" t="s">
+        <v>198</v>
+      </c>
+      <c r="S44">
+        <v>10796</v>
+      </c>
+      <c r="T44" t="s">
+        <v>199</v>
+      </c>
+      <c r="U44" t="s">
+        <v>200</v>
+      </c>
+      <c r="V44" t="s">
+        <v>157</v>
+      </c>
+      <c r="W44" t="s">
+        <v>60</v>
+      </c>
+      <c r="X44" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y44" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>203</v>
+      </c>
+      <c r="B45" t="s">
+        <v>204</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>206</v>
+      </c>
+      <c r="G45" t="s">
+        <v>207</v>
+      </c>
+      <c r="H45" t="s">
+        <v>208</v>
+      </c>
+      <c r="I45" t="s">
+        <v>209</v>
+      </c>
+      <c r="J45" t="s">
+        <v>210</v>
+      </c>
+      <c r="K45" t="s">
+        <v>211</v>
+      </c>
+      <c r="L45" t="s">
+        <v>212</v>
+      </c>
+      <c r="M45">
+        <v>2643743</v>
+      </c>
+      <c r="N45">
+        <v>51.507399999999997</v>
+      </c>
+      <c r="O45">
+        <v>-0.12775800000000001</v>
+      </c>
+      <c r="P45">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>213</v>
+      </c>
+      <c r="R45" t="s">
+        <v>214</v>
+      </c>
+      <c r="S45">
+        <v>5413</v>
+      </c>
+      <c r="T45" t="s">
+        <v>215</v>
+      </c>
+      <c r="U45" t="s">
+        <v>77</v>
+      </c>
+      <c r="V45" t="s">
+        <v>157</v>
+      </c>
+      <c r="W45" t="s">
+        <v>216</v>
+      </c>
+      <c r="X45" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y45" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>218</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>147</v>
+      </c>
+      <c r="G46" t="s">
+        <v>148</v>
+      </c>
+      <c r="H46" t="s">
+        <v>149</v>
+      </c>
+      <c r="I46" t="s">
+        <v>150</v>
+      </c>
+      <c r="J46" t="s">
+        <v>146</v>
+      </c>
+      <c r="K46" t="s">
+        <v>151</v>
+      </c>
+      <c r="L46" t="s">
+        <v>152</v>
+      </c>
+      <c r="M46">
+        <v>1671467</v>
+      </c>
+      <c r="N46">
+        <v>25.068899999999999</v>
+      </c>
+      <c r="O46">
+        <v>121.59099999999999</v>
+      </c>
+      <c r="P46">
+        <v>8</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>153</v>
+      </c>
+      <c r="R46" t="s">
+        <v>154</v>
+      </c>
+      <c r="S46">
+        <v>3462</v>
+      </c>
+      <c r="T46" t="s">
+        <v>155</v>
+      </c>
+      <c r="U46" t="s">
+        <v>156</v>
+      </c>
+      <c r="V46" t="s">
+        <v>157</v>
+      </c>
+      <c r="W46" t="s">
+        <v>41</v>
+      </c>
+      <c r="X46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>147</v>
+      </c>
+      <c r="G47" t="s">
+        <v>148</v>
+      </c>
+      <c r="H47" t="s">
+        <v>149</v>
+      </c>
+      <c r="I47" t="s">
+        <v>150</v>
+      </c>
+      <c r="J47" t="s">
+        <v>146</v>
+      </c>
+      <c r="K47" t="s">
+        <v>151</v>
+      </c>
+      <c r="L47" t="s">
+        <v>152</v>
+      </c>
+      <c r="M47">
+        <v>1671467</v>
+      </c>
+      <c r="N47">
+        <v>25.068899999999999</v>
+      </c>
+      <c r="O47">
+        <v>121.59099999999999</v>
+      </c>
+      <c r="P47">
+        <v>8</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>153</v>
+      </c>
+      <c r="R47" t="s">
+        <v>154</v>
+      </c>
+      <c r="S47">
+        <v>3462</v>
+      </c>
+      <c r="T47" t="s">
+        <v>155</v>
+      </c>
+      <c r="U47" t="s">
+        <v>156</v>
+      </c>
+      <c r="V47" t="s">
+        <v>157</v>
+      </c>
+      <c r="W47" t="s">
+        <v>41</v>
+      </c>
+      <c r="X47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" t="s">
+        <v>219</v>
+      </c>
+      <c r="D48" t="s">
+        <v>220</v>
+      </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>221</v>
+      </c>
+      <c r="G48" t="s">
+        <v>148</v>
+      </c>
+      <c r="H48" t="s">
+        <v>222</v>
+      </c>
+      <c r="I48" t="s">
+        <v>223</v>
+      </c>
+      <c r="L48" t="s">
+        <v>224</v>
+      </c>
+      <c r="M48">
+        <v>1880252</v>
+      </c>
+      <c r="N48">
+        <v>1.3212299999999999</v>
+      </c>
+      <c r="O48">
+        <v>103.69499999999999</v>
+      </c>
+      <c r="P48">
+        <v>8</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>225</v>
+      </c>
+      <c r="R48" t="s">
+        <v>226</v>
+      </c>
+      <c r="S48">
+        <v>14061</v>
+      </c>
+      <c r="T48" t="s">
+        <v>227</v>
+      </c>
+      <c r="U48" t="s">
+        <v>228</v>
+      </c>
+      <c r="V48" t="s">
+        <v>229</v>
+      </c>
+      <c r="W48" t="s">
+        <v>228</v>
+      </c>
+      <c r="X48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC48" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" t="s">
+        <v>161</v>
+      </c>
+      <c r="H49" t="s">
+        <v>162</v>
+      </c>
+      <c r="I49" t="s">
+        <v>163</v>
+      </c>
+      <c r="J49" t="s">
+        <v>164</v>
+      </c>
+      <c r="K49" t="s">
+        <v>165</v>
+      </c>
+      <c r="L49" t="s">
+        <v>166</v>
+      </c>
+      <c r="M49">
+        <v>1606640</v>
+      </c>
+      <c r="N49">
+        <v>13.726699999999999</v>
+      </c>
+      <c r="O49">
+        <v>100.515</v>
+      </c>
+      <c r="P49">
+        <v>7</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>167</v>
+      </c>
+      <c r="R49" t="s">
+        <v>168</v>
+      </c>
+      <c r="S49">
+        <v>131090</v>
+      </c>
+      <c r="T49" t="s">
+        <v>169</v>
+      </c>
+      <c r="U49" t="s">
+        <v>170</v>
+      </c>
+      <c r="V49" t="s">
+        <v>157</v>
+      </c>
+      <c r="X49" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y49" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC49" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" t="s">
+        <v>146</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>147</v>
+      </c>
+      <c r="G50" t="s">
+        <v>148</v>
+      </c>
+      <c r="H50" t="s">
+        <v>149</v>
+      </c>
+      <c r="I50" t="s">
+        <v>150</v>
+      </c>
+      <c r="J50" t="s">
+        <v>146</v>
+      </c>
+      <c r="K50" t="s">
+        <v>151</v>
+      </c>
+      <c r="L50" t="s">
+        <v>231</v>
+      </c>
+      <c r="M50">
+        <v>1668341</v>
+      </c>
+      <c r="N50">
+        <v>25.0334</v>
+      </c>
+      <c r="O50">
+        <v>121.566</v>
+      </c>
+      <c r="P50">
+        <v>8</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>153</v>
+      </c>
+      <c r="R50" t="s">
+        <v>232</v>
+      </c>
+      <c r="S50">
+        <v>3462</v>
+      </c>
+      <c r="T50" t="s">
+        <v>155</v>
+      </c>
+      <c r="U50" t="s">
+        <v>156</v>
+      </c>
+      <c r="V50" t="s">
+        <v>157</v>
+      </c>
+      <c r="W50" t="s">
+        <v>41</v>
+      </c>
+      <c r="X50" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y50" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC50" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>147</v>
+      </c>
+      <c r="G51" t="s">
+        <v>148</v>
+      </c>
+      <c r="H51" t="s">
+        <v>149</v>
+      </c>
+      <c r="I51" t="s">
+        <v>150</v>
+      </c>
+      <c r="J51" t="s">
+        <v>146</v>
+      </c>
+      <c r="K51" t="s">
+        <v>151</v>
+      </c>
+      <c r="L51" t="s">
+        <v>231</v>
+      </c>
+      <c r="M51">
+        <v>1668341</v>
+      </c>
+      <c r="N51">
+        <v>25.0334</v>
+      </c>
+      <c r="O51">
+        <v>121.566</v>
+      </c>
+      <c r="P51">
+        <v>8</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>153</v>
+      </c>
+      <c r="R51" t="s">
+        <v>232</v>
+      </c>
+      <c r="S51">
+        <v>3462</v>
+      </c>
+      <c r="T51" t="s">
+        <v>155</v>
+      </c>
+      <c r="U51" t="s">
+        <v>156</v>
+      </c>
+      <c r="V51" t="s">
+        <v>157</v>
+      </c>
+      <c r="W51" t="s">
+        <v>41</v>
+      </c>
+      <c r="X51" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>147</v>
+      </c>
+      <c r="G52" t="s">
+        <v>148</v>
+      </c>
+      <c r="H52" t="s">
+        <v>149</v>
+      </c>
+      <c r="I52" t="s">
+        <v>150</v>
+      </c>
+      <c r="J52" t="s">
+        <v>146</v>
+      </c>
+      <c r="K52" t="s">
+        <v>151</v>
+      </c>
+      <c r="L52" t="s">
+        <v>152</v>
+      </c>
+      <c r="M52">
+        <v>1671467</v>
+      </c>
+      <c r="N52">
+        <v>25.068899999999999</v>
+      </c>
+      <c r="O52">
+        <v>121.59099999999999</v>
+      </c>
+      <c r="P52">
+        <v>8</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>153</v>
+      </c>
+      <c r="R52" t="s">
+        <v>154</v>
+      </c>
+      <c r="S52">
+        <v>3462</v>
+      </c>
+      <c r="T52" t="s">
+        <v>155</v>
+      </c>
+      <c r="U52" t="s">
+        <v>156</v>
+      </c>
+      <c r="V52" t="s">
+        <v>157</v>
+      </c>
+      <c r="W52" t="s">
+        <v>41</v>
+      </c>
+      <c r="X52" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y52" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
+        <v>146</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>147</v>
+      </c>
+      <c r="G53" t="s">
+        <v>148</v>
+      </c>
+      <c r="H53" t="s">
+        <v>149</v>
+      </c>
+      <c r="I53" t="s">
+        <v>150</v>
+      </c>
+      <c r="J53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K53" t="s">
+        <v>151</v>
+      </c>
+      <c r="L53" t="s">
+        <v>231</v>
+      </c>
+      <c r="M53">
+        <v>1668341</v>
+      </c>
+      <c r="N53">
+        <v>25.0334</v>
+      </c>
+      <c r="O53">
+        <v>121.566</v>
+      </c>
+      <c r="P53">
+        <v>8</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>153</v>
+      </c>
+      <c r="R53" t="s">
+        <v>232</v>
+      </c>
+      <c r="S53">
+        <v>3462</v>
+      </c>
+      <c r="T53" t="s">
+        <v>155</v>
+      </c>
+      <c r="U53" t="s">
+        <v>156</v>
+      </c>
+      <c r="V53" t="s">
+        <v>157</v>
+      </c>
+      <c r="W53" t="s">
+        <v>41</v>
+      </c>
+      <c r="X53" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y53" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B1">
+  <autoFilter ref="A1:B1" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>